<commit_message>
2023.8.3 21.40 model add
</commit_message>
<xml_diff>
--- a/参考/参考/资料/1.18版本策划.xlsx
+++ b/参考/参考/资料/1.18版本策划.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hqyzsy\IdeaProjects\micro_machinery\参考\参考\资料\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73D7D0CA-B4A8-49B8-8382-B5A7DA135651}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FE381CC-E31D-44D1-8B24-0C906EF1BA0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="新增方块" sheetId="1" r:id="rId1"/>
@@ -836,7 +836,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="976" uniqueCount="845">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="976" uniqueCount="846">
   <si>
     <t>矿石</t>
   </si>
@@ -4078,6 +4078,10 @@
   </si>
   <si>
     <t>iron_hammer</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>electrolysis</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -4300,7 +4304,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -4319,6 +4323,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -4332,7 +4342,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -4479,6 +4489,15 @@
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -5807,8 +5826,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B1:AP28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="V1" workbookViewId="0">
-      <selection activeCell="AP17" sqref="AP17"/>
+    <sheetView topLeftCell="V1" workbookViewId="0">
+      <selection activeCell="AD24" sqref="AD24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.640625" defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
@@ -7170,8 +7189,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B1:L15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7:E7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.640625" defaultRowHeight="14.6" x14ac:dyDescent="0.35"/>
@@ -7221,7 +7240,7 @@
       </c>
     </row>
     <row r="2" spans="2:12" ht="28.3" x14ac:dyDescent="0.35">
-      <c r="B2" s="34" t="s">
+      <c r="B2" s="51" t="s">
         <v>361</v>
       </c>
       <c r="C2" s="35" t="s">
@@ -7247,7 +7266,7 @@
       </c>
     </row>
     <row r="3" spans="2:12" ht="28.3" x14ac:dyDescent="0.35">
-      <c r="B3" s="38" t="s">
+      <c r="B3" s="52" t="s">
         <v>570</v>
       </c>
       <c r="C3" s="35" t="s">
@@ -7273,7 +7292,7 @@
       </c>
     </row>
     <row r="4" spans="2:12" ht="28.3" x14ac:dyDescent="0.35">
-      <c r="B4" s="38" t="s">
+      <c r="B4" s="52" t="s">
         <v>571</v>
       </c>
       <c r="C4" s="35" t="s">
@@ -7331,7 +7350,7 @@
       </c>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="53" t="s">
         <v>373</v>
       </c>
       <c r="C7" s="35" t="s">
@@ -7358,11 +7377,11 @@
       </c>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="53" t="s">
         <v>375</v>
       </c>
       <c r="C8" s="35" t="s">
-        <v>376</v>
+        <v>845</v>
       </c>
       <c r="D8" s="24" t="s">
         <v>601</v>
@@ -7436,14 +7455,14 @@
       </c>
     </row>
     <row r="11" spans="2:12" ht="99" x14ac:dyDescent="0.35">
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="53" t="s">
         <v>384</v>
       </c>
       <c r="C11" s="35" t="s">
         <v>385</v>
       </c>
-      <c r="D11" s="6" t="s">
-        <v>371</v>
+      <c r="D11" s="24" t="s">
+        <v>601</v>
       </c>
       <c r="E11" s="24" t="s">
         <v>658</v>
@@ -7526,6 +7545,7 @@
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>